<commit_message>
adding line to web app users
</commit_message>
<xml_diff>
--- a/translations/in-store/csvContent.xlsx
+++ b/translations/in-store/csvContent.xlsx
@@ -677,12 +677,6 @@
     <t>In-Store Support</t>
   </si>
   <si>
-    <t>Your location provides a service from Amazon that allows customers to ship orders to your location and pick them up. Here you'll learn how to use the App, how to get support and how to provide a best-in-class service to your customers.</t>
-  </si>
-  <si>
-    <t>Tu ubicación ofrece un servicio de Amazon que permite a los clientes enviar pedidos a tu ubicación y recogerlos. Aquí aprenderá cómo usar la aplicación, cómo obtener soporte y cómo brindar el mejor servicio de su clase a sus clientes.</t>
-  </si>
-  <si>
     <t>Content overview</t>
   </si>
   <si>
@@ -1157,9 +1151,6 @@
     <t>Qu'est-ce que le service Amazon Counter ?</t>
   </si>
   <si>
-    <t>L'emplacement de votre commerce fournit un service d'Amazon qui permet aux clients d'expédier des commandes dans votre commerce et de les récupérer. Vous apprendrez ici comment utiliser l'application, comment obtenir de l'aide et comment fournir un service de qualité à vos clients.</t>
-  </si>
-  <si>
     <t>Résumé de la formation</t>
   </si>
   <si>
@@ -1826,9 +1817,6 @@
     <t>Bitte folgen Sie dem regulären Prozess bei der Kundenabholung. Durch den Scan des Abholcodes des Kunden, sowie des Pakets, wird die Paketabholung automatisch storniert.</t>
   </si>
   <si>
-    <t>The Amazon Hub Counter Service allows your location to offer customers a new way to receive their orders. Here you’ll learn how to use the App, how to get support and how to provide a best-in-class service to your customers.</t>
-  </si>
-  <si>
     <t>Customers will select your location for pick up at checkout then a driver will deliver those parcels to your location. It is important to scan each parcel in from the driver as soon as possible your scan triggers the customer notification. The customer will have 14 days to pick up the parcel.</t>
   </si>
   <si>
@@ -1854,6 +1842,18 @@
   </si>
   <si>
     <t>//invis.io/U91141V86CGD</t>
+  </si>
+  <si>
+    <t>Your location provides a service from Amazon that allows customers to ship orders to your location and pick them up. Here you'll learn how to use the App, how to get support and how to provide a best-in-class service to your customers. This platform in also valid for web app users.</t>
+  </si>
+  <si>
+    <t>The Amazon Hub Counter Service allows your location to offer customers a new way to receive their orders. Here you’ll learn how to use the App, how to get support and how to provide a best-in-class service to your customers. This platform in also valid for web app users.</t>
+  </si>
+  <si>
+    <t>Tu ubicación ofrece un servicio de Amazon que permite a los clientes enviar pedidos a tu ubicación y recogerlos. Aquí aprenderá cómo usar la aplicación, cómo obtener soporte y cómo brindar el mejor servicio de su clase a sus clientes. Esta plataforma es válida tambíen para web app.</t>
+  </si>
+  <si>
+    <t>L'emplacement de votre commerce fournit un service d'Amazon qui permet aux clients d'expédier des commandes dans votre commerce et de les récupérer. Vous apprendrez ici comment utiliser l'application, comment obtenir de l'aide et comment fournir un service de qualité à vos clients. Cette plateforme est également valable pour les utilisateurs d'applications web.</t>
   </si>
 </sst>
 </file>
@@ -2277,8 +2277,8 @@
   <dimension ref="A1:Q96"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2297,10 +2297,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -2315,16 +2315,16 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -2356,13 +2356,13 @@
         <v>216</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>216</v>
@@ -2397,13 +2397,13 @@
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>6</v>
@@ -2415,39 +2415,39 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="265.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="312.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>217</v>
+        <v>606</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>217</v>
+        <v>606</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>218</v>
+        <v>608</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>218</v>
+        <v>608</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>377</v>
+        <v>609</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -2461,13 +2461,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
@@ -2476,19 +2476,19 @@
         <v>11</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2499,7 +2499,7 @@
     </row>
     <row r="6" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -2517,16 +2517,16 @@
         <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>12</v>
@@ -2543,13 +2543,13 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -2561,16 +2561,16 @@
         <v>17</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -2602,13 +2602,13 @@
         <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>19</v>
@@ -2643,13 +2643,13 @@
         <v>25</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>23</v>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="10" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>26</v>
@@ -2684,13 +2684,13 @@
         <v>28</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>26</v>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="11" spans="1:17" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>29</v>
@@ -2725,13 +2725,13 @@
         <v>31</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>29</v>
@@ -2745,7 +2745,7 @@
     </row>
     <row r="12" spans="1:17" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>32</v>
@@ -2766,13 +2766,13 @@
         <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>32</v>
@@ -2786,37 +2786,37 @@
     </row>
     <row r="13" spans="1:17" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -2827,37 +2827,37 @@
     </row>
     <row r="14" spans="1:17" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="F14" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -2868,37 +2868,37 @@
     </row>
     <row r="15" spans="1:17" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -2909,37 +2909,37 @@
     </row>
     <row r="16" spans="1:17" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -2968,16 +2968,16 @@
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>12</v>
@@ -3012,13 +3012,13 @@
         <v>17</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>15</v>
@@ -3030,18 +3030,18 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="1:17" ht="343.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="328.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>37</v>
@@ -3050,19 +3050,19 @@
         <v>37</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -3076,13 +3076,13 @@
         <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>39</v>
@@ -3091,19 +3091,19 @@
         <v>39</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -3117,13 +3117,13 @@
         <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>41</v>
@@ -3132,19 +3132,19 @@
         <v>41</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -3158,34 +3158,34 @@
         <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3194,39 +3194,39 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="1:17" ht="328.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="297" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3235,7 +3235,7 @@
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
     </row>
-    <row r="24" spans="1:17" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -3255,16 +3255,16 @@
         <v>46</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>45</v>
@@ -3281,34 +3281,34 @@
         <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -3337,16 +3337,16 @@
         <v>50</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>49</v>
@@ -3381,13 +3381,13 @@
         <v>54</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>52</v>
@@ -3422,16 +3422,16 @@
         <v>58</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -3460,16 +3460,16 @@
         <v>61</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>60</v>
@@ -3483,37 +3483,37 @@
     </row>
     <row r="30" spans="1:17" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -3524,37 +3524,37 @@
     </row>
     <row r="31" spans="1:17" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>246</v>
-      </c>
       <c r="H31" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -3565,37 +3565,37 @@
     </row>
     <row r="32" spans="1:17" ht="141" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>62</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -3606,16 +3606,16 @@
     </row>
     <row r="33" spans="1:17" ht="234.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>63</v>
@@ -3624,19 +3624,19 @@
         <v>63</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -3647,37 +3647,37 @@
     </row>
     <row r="34" spans="1:17" ht="297" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -3691,34 +3691,34 @@
         <v>64</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -3750,13 +3750,13 @@
         <v>21</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>66</v>
@@ -3773,34 +3773,34 @@
         <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>550</v>
       </c>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -3814,13 +3814,13 @@
         <v>68</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>39</v>
@@ -3829,19 +3829,19 @@
         <v>39</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -3873,13 +3873,13 @@
         <v>72</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>70</v>
@@ -3911,16 +3911,16 @@
         <v>75</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>74</v>
@@ -3955,13 +3955,13 @@
         <v>79</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>77</v>
@@ -3973,7 +3973,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>80</v>
       </c>
@@ -3996,13 +3996,13 @@
         <v>83</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>81</v>
@@ -4034,16 +4034,16 @@
         <v>86</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>85</v>
@@ -4075,16 +4075,16 @@
         <v>61</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>60</v>
@@ -4098,7 +4098,7 @@
     </row>
     <row r="45" spans="1:17" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>88</v>
@@ -4119,13 +4119,13 @@
         <v>72</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>88</v>
@@ -4139,16 +4139,16 @@
     </row>
     <row r="46" spans="1:17" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>89</v>
@@ -4157,19 +4157,19 @@
         <v>89</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -4180,16 +4180,16 @@
     </row>
     <row r="47" spans="1:17" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>90</v>
@@ -4198,19 +4198,19 @@
         <v>90</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -4221,16 +4221,16 @@
     </row>
     <row r="48" spans="1:17" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>91</v>
@@ -4239,19 +4239,19 @@
         <v>91</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="49" spans="1:17" ht="141" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>92</v>
@@ -4280,16 +4280,16 @@
         <v>93</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>92</v>
@@ -4303,37 +4303,37 @@
     </row>
     <row r="50" spans="1:17" ht="297" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -4342,7 +4342,7 @@
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
     </row>
-    <row r="51" spans="1:17" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>94</v>
       </c>
@@ -4362,16 +4362,16 @@
         <v>96</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>95</v>
@@ -4406,13 +4406,13 @@
         <v>100</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>98</v>
@@ -4447,13 +4447,13 @@
         <v>104</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>102</v>
@@ -4485,16 +4485,16 @@
         <v>107</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>106</v>
@@ -4513,28 +4513,28 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -4566,13 +4566,13 @@
         <v>25</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>109</v>
@@ -4584,39 +4584,39 @@
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
     </row>
-    <row r="57" spans="1:17" ht="406.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="390.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -4630,13 +4630,13 @@
         <v>112</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>39</v>
@@ -4645,19 +4645,19 @@
         <v>39</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -4689,13 +4689,13 @@
         <v>116</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>114</v>
@@ -4727,16 +4727,16 @@
         <v>119</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>118</v>
@@ -4753,13 +4753,13 @@
         <v>120</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>121</v>
@@ -4768,19 +4768,19 @@
         <v>121</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -4812,13 +4812,13 @@
         <v>125</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>123</v>
@@ -4830,18 +4830,18 @@
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
     </row>
-    <row r="63" spans="1:17" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>127</v>
@@ -4850,19 +4850,19 @@
         <v>127</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -4891,16 +4891,16 @@
         <v>130</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>129</v>
@@ -4917,13 +4917,13 @@
         <v>131</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>132</v>
@@ -4932,19 +4932,19 @@
         <v>132</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
@@ -4973,16 +4973,16 @@
         <v>135</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>134</v>
@@ -4999,34 +4999,34 @@
         <v>64</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
@@ -5058,13 +5058,13 @@
         <v>28</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>26</v>
@@ -5076,18 +5076,18 @@
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
     </row>
-    <row r="69" spans="1:17" ht="219" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" ht="203.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>138</v>
@@ -5096,19 +5096,19 @@
         <v>138</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
@@ -5137,16 +5137,16 @@
         <v>141</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>140</v>
@@ -5163,13 +5163,13 @@
         <v>142</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>143</v>
@@ -5178,19 +5178,19 @@
         <v>143</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -5219,16 +5219,16 @@
         <v>146</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>145</v>
@@ -5245,34 +5245,34 @@
         <v>147</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
@@ -5281,7 +5281,7 @@
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>148</v>
       </c>
@@ -5301,16 +5301,16 @@
         <v>150</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>149</v>
@@ -5345,13 +5345,13 @@
         <v>31</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>152</v>
@@ -5368,13 +5368,13 @@
         <v>154</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>155</v>
@@ -5383,19 +5383,19 @@
         <v>155</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
@@ -5424,16 +5424,16 @@
         <v>158</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>157</v>
@@ -5450,13 +5450,13 @@
         <v>159</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>160</v>
@@ -5465,19 +5465,19 @@
         <v>160</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
@@ -5491,13 +5491,13 @@
         <v>161</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>162</v>
@@ -5506,19 +5506,19 @@
         <v>162</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
@@ -5550,13 +5550,13 @@
         <v>166</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>164</v>
@@ -5591,13 +5591,13 @@
         <v>170</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>168</v>
@@ -5609,39 +5609,39 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="E82" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="G82" s="1" t="s">
+      <c r="J82" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="H82" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="J82" s="1" t="s">
-        <v>590</v>
-      </c>
       <c r="K82" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
@@ -5673,13 +5673,13 @@
         <v>175</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>173</v>
@@ -5711,16 +5711,16 @@
         <v>178</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>177</v>
@@ -5755,13 +5755,13 @@
         <v>182</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>180</v>
@@ -5796,13 +5796,13 @@
         <v>186</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>184</v>
@@ -5837,13 +5837,13 @@
         <v>190</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>188</v>
@@ -5875,16 +5875,16 @@
         <v>193</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>192</v>
@@ -5919,13 +5919,13 @@
         <v>197</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>195</v>
@@ -5942,34 +5942,34 @@
         <v>198</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="H90" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="E90" s="1" t="s">
+      <c r="I90" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>589</v>
-      </c>
       <c r="J90" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="L90" s="1"/>
       <c r="M90" s="1"/>
@@ -6001,13 +6001,13 @@
         <v>202</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K91" s="1" t="s">
         <v>200</v>
@@ -6024,34 +6024,34 @@
         <v>203</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="H92" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>585</v>
-      </c>
-      <c r="E92" s="1" t="s">
+      <c r="I92" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="F92" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>589</v>
-      </c>
       <c r="J92" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="L92" s="1"/>
       <c r="M92" s="1"/>
@@ -6083,13 +6083,13 @@
         <v>207</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>205</v>
@@ -6106,13 +6106,13 @@
         <v>208</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>209</v>
@@ -6121,19 +6121,19 @@
         <v>209</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="L94" s="1"/>
       <c r="M94" s="1"/>
@@ -6162,16 +6162,16 @@
         <v>212</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>211</v>
@@ -6188,13 +6188,13 @@
         <v>213</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>214</v>
@@ -6203,19 +6203,19 @@
         <v>214</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>

</xml_diff>